<commit_message>
First stage xlsx -> list(routes) implemented
</commit_message>
<xml_diff>
--- a/TrainRoute.xlsx
+++ b/TrainRoute.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="28695" windowHeight="12540"/>
@@ -2976,8 +2976,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3166,7 +3166,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -3201,7 +3200,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -3377,14 +3375,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A405" workbookViewId="0">
+      <selection activeCell="C435" sqref="C435"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" style="3" customWidth="1"/>
     <col min="2" max="4" width="18" style="3" customWidth="1"/>
@@ -3402,7 +3400,7 @@
     <col min="16" max="16" width="12.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="15.75">
       <c r="A1" s="2" t="s">
         <v>984</v>
       </c>
@@ -3454,7 +3452,7 @@
       <c r="R1" s="8"/>
       <c r="S1" s="8"/>
     </row>
-    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="15.75">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -3499,7 +3497,7 @@
       <c r="R2" s="9"/>
       <c r="S2" s="9"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -3541,7 +3539,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -3583,7 +3581,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
@@ -3625,7 +3623,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="15.75">
       <c r="A6" s="3" t="s">
         <v>20</v>
       </c>
@@ -3667,7 +3665,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="15.75">
       <c r="A7" s="3" t="s">
         <v>25</v>
       </c>
@@ -3709,7 +3707,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="15.75">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -3751,7 +3749,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="15.75">
       <c r="A9" s="3" t="s">
         <v>32</v>
       </c>
@@ -3793,7 +3791,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15.75">
       <c r="A10" s="3" t="s">
         <v>37</v>
       </c>
@@ -3835,7 +3833,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15.75">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -3877,7 +3875,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15.75">
       <c r="A12" s="3" t="s">
         <v>42</v>
       </c>
@@ -3919,7 +3917,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15.75">
       <c r="A13" s="3" t="s">
         <v>49</v>
       </c>
@@ -3961,7 +3959,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15.75">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
@@ -4003,7 +4001,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15.75">
       <c r="A15" s="3" t="s">
         <v>57</v>
       </c>
@@ -4045,7 +4043,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15.75">
       <c r="A16" s="3" t="s">
         <v>58</v>
       </c>
@@ -4087,7 +4085,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="15.75">
       <c r="A17" s="3" t="s">
         <v>59</v>
       </c>
@@ -4132,7 +4130,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15.75">
       <c r="A18" s="3" t="s">
         <v>67</v>
       </c>
@@ -4174,7 +4172,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15.75">
       <c r="A19" s="3" t="s">
         <v>68</v>
       </c>
@@ -4216,7 +4214,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15.75">
       <c r="A20" s="3" t="s">
         <v>69</v>
       </c>
@@ -4258,7 +4256,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15.75">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
@@ -4300,7 +4298,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15.75">
       <c r="A22" s="3" t="s">
         <v>71</v>
       </c>
@@ -4342,7 +4340,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15.75">
       <c r="A23" s="3" t="s">
         <v>72</v>
       </c>
@@ -4384,7 +4382,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15.75">
       <c r="A24" s="3" t="s">
         <v>73</v>
       </c>
@@ -4426,7 +4424,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="15.75">
       <c r="A25" s="3" t="s">
         <v>74</v>
       </c>
@@ -4471,7 +4469,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="15.75">
       <c r="A26" s="3" t="s">
         <v>76</v>
       </c>
@@ -4513,7 +4511,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="15.75">
       <c r="A27" s="3" t="s">
         <v>78</v>
       </c>
@@ -4555,7 +4553,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="15.75">
       <c r="A28" s="3" t="s">
         <v>79</v>
       </c>
@@ -4597,7 +4595,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15.75">
       <c r="A29" s="3" t="s">
         <v>80</v>
       </c>
@@ -4639,7 +4637,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15.75">
       <c r="A30" s="3" t="s">
         <v>81</v>
       </c>
@@ -4681,7 +4679,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15.75">
       <c r="A31" s="3" t="s">
         <v>82</v>
       </c>
@@ -4723,7 +4721,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="15.75">
       <c r="A32" s="3" t="s">
         <v>83</v>
       </c>
@@ -4765,7 +4763,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="15.75">
       <c r="A33" s="3" t="s">
         <v>84</v>
       </c>
@@ -4807,7 +4805,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="15.75">
       <c r="A34" s="3" t="s">
         <v>92</v>
       </c>
@@ -4849,7 +4847,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="15.75">
       <c r="A35" s="3" t="s">
         <v>93</v>
       </c>
@@ -4891,7 +4889,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" ht="15.75">
       <c r="A36" s="3" t="s">
         <v>94</v>
       </c>
@@ -4933,7 +4931,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="15.75">
       <c r="A37" s="3" t="s">
         <v>95</v>
       </c>
@@ -4975,7 +4973,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="15.75">
       <c r="A38" s="3" t="s">
         <v>96</v>
       </c>
@@ -5017,7 +5015,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="15.75">
       <c r="A39" s="3" t="s">
         <v>97</v>
       </c>
@@ -5059,7 +5057,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="15.75">
       <c r="A40" s="3" t="s">
         <v>98</v>
       </c>
@@ -5101,7 +5099,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="15.75">
       <c r="A41" s="3" t="s">
         <v>99</v>
       </c>
@@ -5146,7 +5144,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" ht="15.75">
       <c r="A42" s="3" t="s">
         <v>135</v>
       </c>
@@ -5188,7 +5186,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="15.75">
       <c r="A43" s="3" t="s">
         <v>136</v>
       </c>
@@ -5230,7 +5228,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" ht="15.75">
       <c r="A44" s="3" t="s">
         <v>137</v>
       </c>
@@ -5272,7 +5270,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" ht="15.75">
       <c r="A45" s="3" t="s">
         <v>138</v>
       </c>
@@ -5314,7 +5312,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" ht="15.75">
       <c r="A46" s="3" t="s">
         <v>139</v>
       </c>
@@ -5356,7 +5354,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" ht="15.75">
       <c r="A47" s="3" t="s">
         <v>110</v>
       </c>
@@ -5398,7 +5396,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" ht="15.75">
       <c r="A48" s="3" t="s">
         <v>111</v>
       </c>
@@ -5440,7 +5438,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="15.75">
       <c r="A49" s="3" t="s">
         <v>140</v>
       </c>
@@ -5482,7 +5480,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" ht="15.75">
       <c r="A50" s="3" t="s">
         <v>141</v>
       </c>
@@ -5524,7 +5522,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" ht="15.75">
       <c r="A51" s="3" t="s">
         <v>142</v>
       </c>
@@ -5566,7 +5564,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" ht="15.75">
       <c r="A52" s="3" t="s">
         <v>143</v>
       </c>
@@ -5608,7 +5606,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="15.75">
       <c r="A53" s="3" t="s">
         <v>144</v>
       </c>
@@ -5650,7 +5648,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" ht="15.75">
       <c r="A54" s="3" t="s">
         <v>123</v>
       </c>
@@ -5692,7 +5690,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" ht="15.75">
       <c r="A55" s="3" t="s">
         <v>124</v>
       </c>
@@ -5734,7 +5732,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="15.75">
       <c r="A56" s="3" t="s">
         <v>145</v>
       </c>
@@ -5776,7 +5774,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="15.75">
       <c r="A57" s="3" t="s">
         <v>146</v>
       </c>
@@ -5818,7 +5816,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="15.75">
       <c r="A58" s="3" t="s">
         <v>147</v>
       </c>
@@ -5860,7 +5858,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" ht="15.75">
       <c r="A59" s="3" t="s">
         <v>148</v>
       </c>
@@ -5902,7 +5900,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" ht="15.75">
       <c r="A60" s="3" t="s">
         <v>149</v>
       </c>
@@ -5944,7 +5942,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" ht="15.75">
       <c r="A61" s="3" t="s">
         <v>131</v>
       </c>
@@ -5989,7 +5987,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" ht="15.75">
       <c r="A62" s="3" t="s">
         <v>132</v>
       </c>
@@ -6034,7 +6032,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" ht="15.75">
       <c r="A63" s="3" t="s">
         <v>150</v>
       </c>
@@ -6079,7 +6077,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="15.75">
       <c r="A64" s="3" t="s">
         <v>151</v>
       </c>
@@ -6124,7 +6122,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" ht="15.75">
       <c r="A65" s="3" t="s">
         <v>152</v>
       </c>
@@ -6169,7 +6167,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" ht="15.75">
       <c r="A66" s="3" t="s">
         <v>153</v>
       </c>
@@ -6214,7 +6212,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" ht="15.75">
       <c r="A67" s="3" t="s">
         <v>154</v>
       </c>
@@ -6259,7 +6257,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" ht="15.75">
       <c r="A68" s="3" t="s">
         <v>167</v>
       </c>
@@ -6304,7 +6302,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" ht="15.75">
       <c r="A69" s="3" t="s">
         <v>168</v>
       </c>
@@ -6349,7 +6347,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" ht="15.75">
       <c r="A70" s="3" t="s">
         <v>169</v>
       </c>
@@ -6394,7 +6392,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" ht="15.75">
       <c r="A71" s="3" t="s">
         <v>175</v>
       </c>
@@ -6436,7 +6434,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" ht="15.75">
       <c r="A72" s="3" t="s">
         <v>176</v>
       </c>
@@ -6478,7 +6476,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" ht="15.75">
       <c r="A73" s="3" t="s">
         <v>177</v>
       </c>
@@ -6520,7 +6518,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" ht="15.75">
       <c r="A74" s="3" t="s">
         <v>178</v>
       </c>
@@ -6562,7 +6560,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" ht="15.75">
       <c r="A75" s="3" t="s">
         <v>181</v>
       </c>
@@ -6604,7 +6602,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" ht="15.75">
       <c r="A76" s="3" t="s">
         <v>182</v>
       </c>
@@ -6646,7 +6644,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" ht="15.75">
       <c r="A77" s="3" t="s">
         <v>183</v>
       </c>
@@ -6688,7 +6686,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" ht="15.75">
       <c r="A78" s="3" t="s">
         <v>184</v>
       </c>
@@ -6730,7 +6728,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" ht="15.75">
       <c r="A79" s="3" t="s">
         <v>185</v>
       </c>
@@ -6772,7 +6770,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" ht="15.75">
       <c r="A80" s="3" t="s">
         <v>186</v>
       </c>
@@ -6814,7 +6812,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="81" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" ht="15.75">
       <c r="A81" s="3" t="s">
         <v>187</v>
       </c>
@@ -6856,7 +6854,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" ht="15.75">
       <c r="A82" s="3" t="s">
         <v>188</v>
       </c>
@@ -6898,7 +6896,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" ht="15.75">
       <c r="A83" s="3" t="s">
         <v>189</v>
       </c>
@@ -6940,7 +6938,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" ht="15.75">
       <c r="A84" s="3" t="s">
         <v>190</v>
       </c>
@@ -6982,7 +6980,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" ht="15.75">
       <c r="A85" s="3" t="s">
         <v>191</v>
       </c>
@@ -7024,7 +7022,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" ht="15.75">
       <c r="A86" s="3" t="s">
         <v>192</v>
       </c>
@@ -7066,7 +7064,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" ht="15.75">
       <c r="A87" s="3" t="s">
         <v>193</v>
       </c>
@@ -7108,7 +7106,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" ht="15.75">
       <c r="A88" s="3" t="s">
         <v>194</v>
       </c>
@@ -7150,7 +7148,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" ht="15.75">
       <c r="A89" s="3" t="s">
         <v>195</v>
       </c>
@@ -7192,7 +7190,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" ht="15.75">
       <c r="A90" s="3" t="s">
         <v>196</v>
       </c>
@@ -7234,7 +7232,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" ht="15.75">
       <c r="A91" s="3" t="s">
         <v>197</v>
       </c>
@@ -7276,7 +7274,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" ht="15.75">
       <c r="A92" s="3" t="s">
         <v>201</v>
       </c>
@@ -7318,7 +7316,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" ht="15.75">
       <c r="A93" s="3" t="s">
         <v>205</v>
       </c>
@@ -7360,7 +7358,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" ht="15.75">
       <c r="A94" s="3" t="s">
         <v>208</v>
       </c>
@@ -7402,7 +7400,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" ht="15.75">
       <c r="A95" s="3" t="s">
         <v>209</v>
       </c>
@@ -7444,7 +7442,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" ht="15.75">
       <c r="A96" s="3" t="s">
         <v>210</v>
       </c>
@@ -7486,7 +7484,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" ht="15.75">
       <c r="A97" s="3" t="s">
         <v>211</v>
       </c>
@@ -7528,7 +7526,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" ht="15.75">
       <c r="A98" s="3" t="s">
         <v>212</v>
       </c>
@@ -7570,7 +7568,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" ht="15.75">
       <c r="A99" s="3" t="s">
         <v>218</v>
       </c>
@@ -7612,7 +7610,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" ht="15.75">
       <c r="A100" s="3" t="s">
         <v>219</v>
       </c>
@@ -7654,7 +7652,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" ht="15.75">
       <c r="A101" s="3" t="s">
         <v>220</v>
       </c>
@@ -7696,7 +7694,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" ht="15.75">
       <c r="A102" s="3" t="s">
         <v>221</v>
       </c>
@@ -7738,7 +7736,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" ht="15.75">
       <c r="A103" s="3" t="s">
         <v>222</v>
       </c>
@@ -7780,7 +7778,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" ht="15.75">
       <c r="A104" s="3" t="s">
         <v>223</v>
       </c>
@@ -7822,7 +7820,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="105" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" ht="15.75">
       <c r="A105" s="3" t="s">
         <v>224</v>
       </c>
@@ -7864,7 +7862,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" ht="15.75">
       <c r="A106" s="3" t="s">
         <v>225</v>
       </c>
@@ -7906,7 +7904,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" ht="15.75">
       <c r="A107" s="3" t="s">
         <v>242</v>
       </c>
@@ -7951,7 +7949,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" ht="15.75">
       <c r="A108" s="3" t="s">
         <v>243</v>
       </c>
@@ -7993,7 +7991,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" ht="15.75">
       <c r="A109" s="3" t="s">
         <v>244</v>
       </c>
@@ -8035,7 +8033,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" ht="15.75">
       <c r="A110" s="3" t="s">
         <v>245</v>
       </c>
@@ -8077,7 +8075,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" ht="15.75">
       <c r="A111" s="3" t="s">
         <v>246</v>
       </c>
@@ -8119,7 +8117,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" ht="15.75">
       <c r="A112" s="3" t="s">
         <v>247</v>
       </c>
@@ -8161,7 +8159,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" ht="15.75">
       <c r="A113" s="3" t="s">
         <v>248</v>
       </c>
@@ -8203,7 +8201,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" ht="15.75">
       <c r="A114" s="3" t="s">
         <v>250</v>
       </c>
@@ -8245,7 +8243,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" ht="15.75">
       <c r="A115" s="3" t="s">
         <v>251</v>
       </c>
@@ -8287,7 +8285,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" ht="15.75">
       <c r="A116" s="3" t="s">
         <v>252</v>
       </c>
@@ -8329,7 +8327,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" ht="15.75">
       <c r="A117" s="3" t="s">
         <v>253</v>
       </c>
@@ -8371,7 +8369,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" ht="15.75">
       <c r="A118" s="3" t="s">
         <v>254</v>
       </c>
@@ -8413,7 +8411,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" ht="15.75">
       <c r="A119" s="3" t="s">
         <v>255</v>
       </c>
@@ -8455,7 +8453,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" ht="15.75">
       <c r="A120" s="3" t="s">
         <v>256</v>
       </c>
@@ -8497,7 +8495,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" ht="15.75">
       <c r="A121" s="3" t="s">
         <v>257</v>
       </c>
@@ -8542,7 +8540,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" ht="15.75">
       <c r="A122" s="3" t="s">
         <v>261</v>
       </c>
@@ -8584,7 +8582,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" ht="15.75">
       <c r="A123" s="3" t="s">
         <v>260</v>
       </c>
@@ -8626,7 +8624,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" ht="15.75">
       <c r="A124" s="3" t="s">
         <v>259</v>
       </c>
@@ -8668,7 +8666,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" ht="15.75">
       <c r="A125" s="3" t="s">
         <v>262</v>
       </c>
@@ -8710,7 +8708,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" ht="15.75">
       <c r="A126" s="3" t="s">
         <v>263</v>
       </c>
@@ -8752,7 +8750,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" ht="15.75">
       <c r="A127" s="3" t="s">
         <v>264</v>
       </c>
@@ -8794,7 +8792,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" ht="15.75">
       <c r="A128" s="3" t="s">
         <v>265</v>
       </c>
@@ -8836,7 +8834,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" ht="15.75">
       <c r="A129" s="3" t="s">
         <v>266</v>
       </c>
@@ -8878,7 +8876,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" ht="15.75">
       <c r="A130" s="3" t="s">
         <v>275</v>
       </c>
@@ -8920,7 +8918,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" ht="15.75">
       <c r="A131" s="3" t="s">
         <v>276</v>
       </c>
@@ -8962,7 +8960,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" ht="15.75">
       <c r="A132" s="3" t="s">
         <v>277</v>
       </c>
@@ -9004,7 +9002,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" ht="15.75">
       <c r="A133" s="3" t="s">
         <v>278</v>
       </c>
@@ -9046,7 +9044,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" ht="15.75">
       <c r="A134" s="3" t="s">
         <v>279</v>
       </c>
@@ -9088,7 +9086,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" ht="15.75">
       <c r="A135" s="3" t="s">
         <v>280</v>
       </c>
@@ -9130,7 +9128,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16">
       <c r="A136" t="s">
         <v>281</v>
       </c>
@@ -9172,7 +9170,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16">
       <c r="A137" t="s">
         <v>282</v>
       </c>
@@ -9217,7 +9215,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" ht="15.75">
       <c r="A138" t="s">
         <v>286</v>
       </c>
@@ -9262,7 +9260,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" ht="15.75">
       <c r="A139" s="3" t="s">
         <v>290</v>
       </c>
@@ -9307,7 +9305,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" ht="15.75">
       <c r="A140" s="3" t="s">
         <v>292</v>
       </c>
@@ -9352,7 +9350,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" ht="15.75">
       <c r="A141" s="3" t="s">
         <v>287</v>
       </c>
@@ -9397,7 +9395,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" ht="15.75">
       <c r="A142" s="3" t="s">
         <v>294</v>
       </c>
@@ -9442,7 +9440,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" ht="15.75">
       <c r="A143" s="3" t="s">
         <v>296</v>
       </c>
@@ -9487,7 +9485,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" ht="15.75">
       <c r="A144" s="3" t="s">
         <v>298</v>
       </c>
@@ -9532,7 +9530,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="145" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" ht="15.75">
       <c r="A145" s="3" t="s">
         <v>300</v>
       </c>
@@ -9577,7 +9575,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="146" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" ht="15.75">
       <c r="A146" s="3" t="s">
         <v>302</v>
       </c>
@@ -9622,7 +9620,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="147" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" ht="15.75">
       <c r="A147" s="3" t="s">
         <v>303</v>
       </c>
@@ -9667,7 +9665,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="148" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" ht="15.75">
       <c r="A148" s="3" t="s">
         <v>304</v>
       </c>
@@ -9712,7 +9710,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="149" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" ht="15.75">
       <c r="A149" s="3" t="s">
         <v>305</v>
       </c>
@@ -9757,7 +9755,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="150" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:16" ht="15.75">
       <c r="A150" s="3" t="s">
         <v>306</v>
       </c>
@@ -9802,7 +9800,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="151" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" ht="15.75">
       <c r="A151" s="3" t="s">
         <v>307</v>
       </c>
@@ -9847,7 +9845,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="152" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" ht="15.75">
       <c r="A152" s="3" t="s">
         <v>308</v>
       </c>
@@ -9892,7 +9890,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="153" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" ht="15.75">
       <c r="A153" s="3" t="s">
         <v>309</v>
       </c>
@@ -9937,7 +9935,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="154" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" ht="15.75">
       <c r="A154" s="3" t="s">
         <v>310</v>
       </c>
@@ -9982,7 +9980,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="155" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" ht="15.75">
       <c r="A155" s="3" t="s">
         <v>311</v>
       </c>
@@ -10027,7 +10025,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="156" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" ht="15.75">
       <c r="A156" s="3" t="s">
         <v>316</v>
       </c>
@@ -10072,7 +10070,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="157" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" ht="15.75">
       <c r="A157" s="5" t="s">
         <v>317</v>
       </c>
@@ -10117,7 +10115,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="158" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" ht="15.75">
       <c r="A158" s="3" t="s">
         <v>321</v>
       </c>
@@ -10142,7 +10140,7 @@
       </c>
       <c r="L158" s="11"/>
     </row>
-    <row r="159" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" ht="15.75">
       <c r="A159" s="3" t="s">
         <v>325</v>
       </c>
@@ -10167,7 +10165,7 @@
       </c>
       <c r="L159" s="11"/>
     </row>
-    <row r="160" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" ht="15.75">
       <c r="A160" s="3" t="s">
         <v>326</v>
       </c>
@@ -10195,7 +10193,7 @@
       </c>
       <c r="L160" s="11"/>
     </row>
-    <row r="161" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:12" ht="15.75">
       <c r="A161" s="3" t="s">
         <v>329</v>
       </c>
@@ -10223,7 +10221,7 @@
       </c>
       <c r="L161" s="11"/>
     </row>
-    <row r="162" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:12" ht="15.75">
       <c r="A162" s="3" t="s">
         <v>334</v>
       </c>
@@ -10251,7 +10249,7 @@
       </c>
       <c r="L162" s="11"/>
     </row>
-    <row r="163" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:12" ht="15.75">
       <c r="A163" s="3" t="s">
         <v>337</v>
       </c>
@@ -10279,7 +10277,7 @@
       </c>
       <c r="L163" s="11"/>
     </row>
-    <row r="164" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:12" ht="15.75">
       <c r="A164" s="3" t="s">
         <v>339</v>
       </c>
@@ -10307,7 +10305,7 @@
       </c>
       <c r="L164" s="11"/>
     </row>
-    <row r="165" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:12" ht="15.75">
       <c r="A165" s="3" t="s">
         <v>343</v>
       </c>
@@ -10335,7 +10333,7 @@
       </c>
       <c r="L165" s="11"/>
     </row>
-    <row r="166" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:12" ht="15.75">
       <c r="A166" s="3" t="s">
         <v>349</v>
       </c>
@@ -10363,7 +10361,7 @@
       </c>
       <c r="L166" s="11"/>
     </row>
-    <row r="167" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:12" ht="15.75">
       <c r="A167" s="3" t="s">
         <v>353</v>
       </c>
@@ -10391,7 +10389,7 @@
       </c>
       <c r="L167" s="11"/>
     </row>
-    <row r="168" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:12" ht="15.75">
       <c r="A168" s="3" t="s">
         <v>355</v>
       </c>
@@ -10419,7 +10417,7 @@
       </c>
       <c r="L168" s="11"/>
     </row>
-    <row r="169" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:12" ht="15.75">
       <c r="A169" s="3" t="s">
         <v>358</v>
       </c>
@@ -10447,7 +10445,7 @@
       </c>
       <c r="L169" s="11"/>
     </row>
-    <row r="170" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:12" ht="15.75">
       <c r="A170" s="3" t="s">
         <v>361</v>
       </c>
@@ -10475,7 +10473,7 @@
       </c>
       <c r="L170" s="11"/>
     </row>
-    <row r="171" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:12" ht="15.75">
       <c r="A171" s="3" t="s">
         <v>364</v>
       </c>
@@ -10503,7 +10501,7 @@
       </c>
       <c r="L171" s="11"/>
     </row>
-    <row r="172" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:12" ht="15.75">
       <c r="A172" s="3" t="s">
         <v>367</v>
       </c>
@@ -10531,7 +10529,7 @@
       </c>
       <c r="L172" s="11"/>
     </row>
-    <row r="173" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:12" ht="15.75">
       <c r="A173" s="3" t="s">
         <v>369</v>
       </c>
@@ -10559,7 +10557,7 @@
       </c>
       <c r="L173" s="11"/>
     </row>
-    <row r="174" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:12" ht="15.75">
       <c r="A174" s="3" t="s">
         <v>370</v>
       </c>
@@ -10587,7 +10585,7 @@
       </c>
       <c r="L174" s="11"/>
     </row>
-    <row r="175" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:12" ht="15.75">
       <c r="A175" s="3" t="s">
         <v>372</v>
       </c>
@@ -10615,7 +10613,7 @@
       </c>
       <c r="L175" s="11"/>
     </row>
-    <row r="176" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:12" ht="15.75">
       <c r="A176" s="3" t="s">
         <v>374</v>
       </c>
@@ -10643,7 +10641,7 @@
       </c>
       <c r="L176" s="11"/>
     </row>
-    <row r="177" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:12" ht="15.75">
       <c r="A177" s="3" t="s">
         <v>377</v>
       </c>
@@ -10671,7 +10669,7 @@
       </c>
       <c r="L177" s="11"/>
     </row>
-    <row r="178" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:12" ht="15.75">
       <c r="A178" s="3" t="s">
         <v>379</v>
       </c>
@@ -10699,7 +10697,7 @@
       </c>
       <c r="L178" s="11"/>
     </row>
-    <row r="179" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:12" ht="15.75">
       <c r="A179" s="3" t="s">
         <v>382</v>
       </c>
@@ -10727,7 +10725,7 @@
       </c>
       <c r="L179" s="11"/>
     </row>
-    <row r="180" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:12" ht="15.75">
       <c r="A180" s="3" t="s">
         <v>385</v>
       </c>
@@ -10755,7 +10753,7 @@
       </c>
       <c r="L180" s="11"/>
     </row>
-    <row r="181" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:12" ht="15.75">
       <c r="A181" s="3" t="s">
         <v>386</v>
       </c>
@@ -10783,7 +10781,7 @@
       </c>
       <c r="L181" s="11"/>
     </row>
-    <row r="182" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:12" ht="15.75">
       <c r="A182" s="3" t="s">
         <v>388</v>
       </c>
@@ -10811,7 +10809,7 @@
       </c>
       <c r="L182" s="11"/>
     </row>
-    <row r="183" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:12" ht="15.75">
       <c r="A183" s="3" t="s">
         <v>389</v>
       </c>
@@ -10839,7 +10837,7 @@
       </c>
       <c r="L183" s="11"/>
     </row>
-    <row r="184" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:12" ht="15.75">
       <c r="A184" s="3" t="s">
         <v>392</v>
       </c>
@@ -10867,7 +10865,7 @@
       </c>
       <c r="L184" s="11"/>
     </row>
-    <row r="185" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:12" ht="15.75">
       <c r="A185" s="3" t="s">
         <v>393</v>
       </c>
@@ -10895,7 +10893,7 @@
       </c>
       <c r="L185" s="11"/>
     </row>
-    <row r="186" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:12" ht="15.75">
       <c r="A186" s="3" t="s">
         <v>395</v>
       </c>
@@ -10923,7 +10921,7 @@
       </c>
       <c r="L186" s="11"/>
     </row>
-    <row r="187" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:12" ht="15.75">
       <c r="A187" s="3" t="s">
         <v>396</v>
       </c>
@@ -10951,7 +10949,7 @@
       </c>
       <c r="L187" s="11"/>
     </row>
-    <row r="188" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:12" ht="15.75">
       <c r="A188" s="3" t="s">
         <v>397</v>
       </c>
@@ -10979,7 +10977,7 @@
       </c>
       <c r="L188" s="11"/>
     </row>
-    <row r="189" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:12" ht="15.75">
       <c r="A189" s="3" t="s">
         <v>400</v>
       </c>
@@ -11007,7 +11005,7 @@
       </c>
       <c r="L189" s="11"/>
     </row>
-    <row r="190" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:12" ht="15.75">
       <c r="A190" s="3" t="s">
         <v>402</v>
       </c>
@@ -11035,7 +11033,7 @@
       </c>
       <c r="L190" s="11"/>
     </row>
-    <row r="191" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:12" ht="15.75">
       <c r="A191" s="3" t="s">
         <v>404</v>
       </c>
@@ -11063,7 +11061,7 @@
       </c>
       <c r="L191" s="11"/>
     </row>
-    <row r="192" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:12" ht="15.75">
       <c r="A192" s="3" t="s">
         <v>408</v>
       </c>
@@ -11091,7 +11089,7 @@
       </c>
       <c r="L192" s="11"/>
     </row>
-    <row r="193" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:12" ht="15.75">
       <c r="A193" s="3" t="s">
         <v>410</v>
       </c>
@@ -11119,7 +11117,7 @@
       </c>
       <c r="L193" s="11"/>
     </row>
-    <row r="194" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:12" ht="15.75">
       <c r="A194" s="3" t="s">
         <v>413</v>
       </c>
@@ -11147,7 +11145,7 @@
       </c>
       <c r="L194" s="11"/>
     </row>
-    <row r="195" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:12" ht="15.75">
       <c r="A195" s="3" t="s">
         <v>414</v>
       </c>
@@ -11175,7 +11173,7 @@
       </c>
       <c r="L195" s="11"/>
     </row>
-    <row r="196" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:12" ht="15.75">
       <c r="A196" s="3" t="s">
         <v>417</v>
       </c>
@@ -11203,7 +11201,7 @@
       </c>
       <c r="L196" s="11"/>
     </row>
-    <row r="197" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:12" ht="15.75">
       <c r="A197" s="3" t="s">
         <v>418</v>
       </c>
@@ -11231,7 +11229,7 @@
       </c>
       <c r="L197" s="11"/>
     </row>
-    <row r="198" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:12" ht="15.75">
       <c r="A198" s="3" t="s">
         <v>419</v>
       </c>
@@ -11259,7 +11257,7 @@
       </c>
       <c r="L198" s="11"/>
     </row>
-    <row r="199" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:12" ht="15.75">
       <c r="A199" s="3" t="s">
         <v>424</v>
       </c>
@@ -11287,7 +11285,7 @@
       </c>
       <c r="L199" s="11"/>
     </row>
-    <row r="200" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:12" ht="15.75">
       <c r="A200" s="3" t="s">
         <v>427</v>
       </c>
@@ -11315,7 +11313,7 @@
       </c>
       <c r="L200" s="11"/>
     </row>
-    <row r="201" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:12" ht="15.75">
       <c r="A201" s="3" t="s">
         <v>430</v>
       </c>
@@ -11343,7 +11341,7 @@
       </c>
       <c r="L201" s="11"/>
     </row>
-    <row r="202" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:12" ht="15.75">
       <c r="A202" s="3" t="s">
         <v>431</v>
       </c>
@@ -11371,7 +11369,7 @@
       </c>
       <c r="L202" s="11"/>
     </row>
-    <row r="203" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:12" ht="15.75">
       <c r="A203" s="3" t="s">
         <v>432</v>
       </c>
@@ -11399,7 +11397,7 @@
       </c>
       <c r="L203" s="11"/>
     </row>
-    <row r="204" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:12" ht="15.75">
       <c r="A204" s="3" t="s">
         <v>434</v>
       </c>
@@ -11427,7 +11425,7 @@
       </c>
       <c r="L204" s="11"/>
     </row>
-    <row r="205" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:12" ht="15.75">
       <c r="A205" s="3" t="s">
         <v>435</v>
       </c>
@@ -11455,7 +11453,7 @@
       </c>
       <c r="L205" s="11"/>
     </row>
-    <row r="206" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:12" ht="15.75">
       <c r="A206" s="3" t="s">
         <v>436</v>
       </c>
@@ -11483,7 +11481,7 @@
       </c>
       <c r="L206" s="11"/>
     </row>
-    <row r="207" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:12" ht="15.75">
       <c r="A207" s="3" t="s">
         <v>438</v>
       </c>
@@ -11511,7 +11509,7 @@
       </c>
       <c r="L207" s="11"/>
     </row>
-    <row r="208" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:12" ht="15.75">
       <c r="A208" s="3" t="s">
         <v>112</v>
       </c>
@@ -11539,7 +11537,7 @@
       </c>
       <c r="L208" s="11"/>
     </row>
-    <row r="209" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:12" ht="15.75">
       <c r="A209" s="3" t="s">
         <v>113</v>
       </c>
@@ -11567,7 +11565,7 @@
       </c>
       <c r="L209" s="11"/>
     </row>
-    <row r="210" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:12" ht="15.75">
       <c r="A210" s="3" t="s">
         <v>442</v>
       </c>
@@ -11595,7 +11593,7 @@
       </c>
       <c r="L210" s="11"/>
     </row>
-    <row r="211" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:12" ht="15.75">
       <c r="A211" s="3" t="s">
         <v>444</v>
       </c>
@@ -11623,7 +11621,7 @@
       </c>
       <c r="L211" s="11"/>
     </row>
-    <row r="212" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:12" ht="15.75">
       <c r="A212" s="3" t="s">
         <v>445</v>
       </c>
@@ -11651,7 +11649,7 @@
       </c>
       <c r="L212" s="11"/>
     </row>
-    <row r="213" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:12" ht="15.75">
       <c r="A213" s="3" t="s">
         <v>446</v>
       </c>
@@ -11679,7 +11677,7 @@
       </c>
       <c r="L213" s="11"/>
     </row>
-    <row r="214" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:12" ht="15.75">
       <c r="A214" s="3" t="s">
         <v>447</v>
       </c>
@@ -11707,7 +11705,7 @@
       </c>
       <c r="L214" s="11"/>
     </row>
-    <row r="215" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:12" ht="15.75">
       <c r="A215" s="3" t="s">
         <v>450</v>
       </c>
@@ -11735,7 +11733,7 @@
       </c>
       <c r="L215" s="11"/>
     </row>
-    <row r="216" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:12" ht="15.75">
       <c r="A216" s="3" t="s">
         <v>451</v>
       </c>
@@ -11763,7 +11761,7 @@
       </c>
       <c r="L216" s="11"/>
     </row>
-    <row r="217" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:12" ht="15.75">
       <c r="A217" s="3" t="s">
         <v>452</v>
       </c>
@@ -11791,7 +11789,7 @@
       </c>
       <c r="L217" s="11"/>
     </row>
-    <row r="218" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:12" ht="15.75">
       <c r="A218" s="3" t="s">
         <v>453</v>
       </c>
@@ -11819,7 +11817,7 @@
       </c>
       <c r="L218" s="11"/>
     </row>
-    <row r="219" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:12" ht="15.75">
       <c r="A219" s="3" t="s">
         <v>458</v>
       </c>
@@ -11847,7 +11845,7 @@
       </c>
       <c r="L219" s="11"/>
     </row>
-    <row r="220" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:12" ht="15.75">
       <c r="A220" s="3" t="s">
         <v>461</v>
       </c>
@@ -11875,7 +11873,7 @@
       </c>
       <c r="L220" s="11"/>
     </row>
-    <row r="221" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:12" ht="15.75">
       <c r="A221" s="3" t="s">
         <v>465</v>
       </c>
@@ -11903,7 +11901,7 @@
       </c>
       <c r="L221" s="11"/>
     </row>
-    <row r="222" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:12" ht="15.75">
       <c r="A222" s="3" t="s">
         <v>467</v>
       </c>
@@ -11931,7 +11929,7 @@
       </c>
       <c r="L222" s="11"/>
     </row>
-    <row r="223" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:12" ht="15.75">
       <c r="A223" s="3" t="s">
         <v>471</v>
       </c>
@@ -11959,7 +11957,7 @@
       </c>
       <c r="L223" s="11"/>
     </row>
-    <row r="224" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:12" ht="15.75">
       <c r="A224" s="3" t="s">
         <v>475</v>
       </c>
@@ -11987,7 +11985,7 @@
       </c>
       <c r="L224" s="11"/>
     </row>
-    <row r="225" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:12" ht="15.75">
       <c r="A225" s="3" t="s">
         <v>478</v>
       </c>
@@ -12015,7 +12013,7 @@
       </c>
       <c r="L225" s="11"/>
     </row>
-    <row r="226" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:12" ht="15.75">
       <c r="A226" s="3" t="s">
         <v>480</v>
       </c>
@@ -12043,7 +12041,7 @@
       </c>
       <c r="L226" s="11"/>
     </row>
-    <row r="227" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:12" ht="15.75">
       <c r="A227" s="3" t="s">
         <v>483</v>
       </c>
@@ -12071,7 +12069,7 @@
       </c>
       <c r="L227" s="11"/>
     </row>
-    <row r="228" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:12" ht="15.75">
       <c r="A228" s="3" t="s">
         <v>485</v>
       </c>
@@ -12099,7 +12097,7 @@
       </c>
       <c r="L228" s="11"/>
     </row>
-    <row r="229" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:12" ht="15.75">
       <c r="A229" s="3" t="s">
         <v>487</v>
       </c>
@@ -12127,7 +12125,7 @@
       </c>
       <c r="L229" s="11"/>
     </row>
-    <row r="230" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:12" ht="15.75">
       <c r="A230" s="3" t="s">
         <v>490</v>
       </c>
@@ -12155,7 +12153,7 @@
       </c>
       <c r="L230" s="11"/>
     </row>
-    <row r="231" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:12" ht="15.75">
       <c r="A231" s="3" t="s">
         <v>491</v>
       </c>
@@ -12183,7 +12181,7 @@
       </c>
       <c r="L231" s="11"/>
     </row>
-    <row r="232" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:12" ht="15.75">
       <c r="A232" s="3" t="s">
         <v>492</v>
       </c>
@@ -12211,7 +12209,7 @@
       </c>
       <c r="L232" s="11"/>
     </row>
-    <row r="233" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:12" ht="15.75">
       <c r="A233" s="3" t="s">
         <v>493</v>
       </c>
@@ -12239,7 +12237,7 @@
       </c>
       <c r="L233" s="11"/>
     </row>
-    <row r="234" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:12" ht="15.75">
       <c r="A234" s="3" t="s">
         <v>499</v>
       </c>
@@ -12267,7 +12265,7 @@
       </c>
       <c r="L234" s="11"/>
     </row>
-    <row r="235" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:12" ht="15.75">
       <c r="A235" s="3" t="s">
         <v>502</v>
       </c>
@@ -12295,7 +12293,7 @@
       </c>
       <c r="L235" s="11"/>
     </row>
-    <row r="236" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:12" ht="15.75">
       <c r="A236" s="3" t="s">
         <v>507</v>
       </c>
@@ -12323,7 +12321,7 @@
       </c>
       <c r="L236" s="11"/>
     </row>
-    <row r="237" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:12" ht="15.75">
       <c r="A237" s="3" t="s">
         <v>508</v>
       </c>
@@ -12351,7 +12349,7 @@
       </c>
       <c r="L237" s="11"/>
     </row>
-    <row r="238" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:12" ht="15.75">
       <c r="A238" s="3" t="s">
         <v>510</v>
       </c>
@@ -12379,7 +12377,7 @@
       </c>
       <c r="L238" s="11"/>
     </row>
-    <row r="239" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:12" ht="15.75">
       <c r="A239" s="3" t="s">
         <v>511</v>
       </c>
@@ -12407,7 +12405,7 @@
       </c>
       <c r="L239" s="11"/>
     </row>
-    <row r="240" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:12" ht="15.75">
       <c r="A240" s="3" t="s">
         <v>513</v>
       </c>
@@ -12435,7 +12433,7 @@
       </c>
       <c r="L240" s="11"/>
     </row>
-    <row r="241" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:12" ht="15.75">
       <c r="A241" s="3" t="s">
         <v>517</v>
       </c>
@@ -12463,7 +12461,7 @@
       </c>
       <c r="L241" s="11"/>
     </row>
-    <row r="242" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:12" ht="15.75">
       <c r="A242" s="3" t="s">
         <v>520</v>
       </c>
@@ -12491,7 +12489,7 @@
       </c>
       <c r="L242" s="11"/>
     </row>
-    <row r="243" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:12" ht="15.75">
       <c r="A243" s="3" t="s">
         <v>524</v>
       </c>
@@ -12519,7 +12517,7 @@
       </c>
       <c r="L243" s="11"/>
     </row>
-    <row r="244" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:12" ht="15.75">
       <c r="A244" s="3" t="s">
         <v>525</v>
       </c>
@@ -12547,7 +12545,7 @@
       </c>
       <c r="L244" s="11"/>
     </row>
-    <row r="245" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:12" ht="15.75">
       <c r="A245" s="3" t="s">
         <v>526</v>
       </c>
@@ -12575,7 +12573,7 @@
       </c>
       <c r="L245" s="11"/>
     </row>
-    <row r="246" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:12" ht="15.75">
       <c r="A246" s="3" t="s">
         <v>527</v>
       </c>
@@ -12603,7 +12601,7 @@
       </c>
       <c r="L246" s="11"/>
     </row>
-    <row r="247" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:12" ht="15.75">
       <c r="A247" s="3" t="s">
         <v>528</v>
       </c>
@@ -12631,7 +12629,7 @@
       </c>
       <c r="L247" s="11"/>
     </row>
-    <row r="248" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:12" ht="15.75">
       <c r="A248" s="3" t="s">
         <v>529</v>
       </c>
@@ -12659,7 +12657,7 @@
       </c>
       <c r="L248" s="11"/>
     </row>
-    <row r="249" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:12" ht="15.75">
       <c r="A249" s="3" t="s">
         <v>530</v>
       </c>
@@ -12687,7 +12685,7 @@
       </c>
       <c r="L249" s="11"/>
     </row>
-    <row r="250" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:12" ht="15.75">
       <c r="A250" s="3" t="s">
         <v>538</v>
       </c>
@@ -12715,7 +12713,7 @@
       </c>
       <c r="L250" s="11"/>
     </row>
-    <row r="251" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:12" ht="15.75">
       <c r="A251" s="3" t="s">
         <v>539</v>
       </c>
@@ -12743,7 +12741,7 @@
       </c>
       <c r="L251" s="11"/>
     </row>
-    <row r="252" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:12" ht="15.75">
       <c r="A252" s="3" t="s">
         <v>540</v>
       </c>
@@ -12771,7 +12769,7 @@
       </c>
       <c r="L252" s="11"/>
     </row>
-    <row r="253" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:12" ht="15.75">
       <c r="A253" s="3" t="s">
         <v>544</v>
       </c>
@@ -12799,7 +12797,7 @@
       </c>
       <c r="L253" s="11"/>
     </row>
-    <row r="254" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:12" ht="15.75">
       <c r="A254" s="3" t="s">
         <v>547</v>
       </c>
@@ -12827,7 +12825,7 @@
       </c>
       <c r="L254" s="11"/>
     </row>
-    <row r="255" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:12" ht="15.75">
       <c r="A255" s="3" t="s">
         <v>549</v>
       </c>
@@ -12855,7 +12853,7 @@
       </c>
       <c r="L255" s="11"/>
     </row>
-    <row r="256" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:12" ht="15.75">
       <c r="A256" s="3" t="s">
         <v>550</v>
       </c>
@@ -12883,7 +12881,7 @@
       </c>
       <c r="L256" s="11"/>
     </row>
-    <row r="257" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:12" ht="15.75">
       <c r="A257" s="3" t="s">
         <v>555</v>
       </c>
@@ -12911,7 +12909,7 @@
       </c>
       <c r="L257" s="11"/>
     </row>
-    <row r="258" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:12" ht="15.75">
       <c r="A258" s="3" t="s">
         <v>556</v>
       </c>
@@ -12939,7 +12937,7 @@
       </c>
       <c r="L258" s="11"/>
     </row>
-    <row r="259" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:12" ht="15.75">
       <c r="A259" s="3" t="s">
         <v>557</v>
       </c>
@@ -12967,7 +12965,7 @@
       </c>
       <c r="L259" s="11"/>
     </row>
-    <row r="260" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:12" ht="15.75">
       <c r="A260" s="3" t="s">
         <v>558</v>
       </c>
@@ -12995,7 +12993,7 @@
       </c>
       <c r="L260" s="11"/>
     </row>
-    <row r="261" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:12" ht="15.75">
       <c r="A261" s="3" t="s">
         <v>559</v>
       </c>
@@ -13023,7 +13021,7 @@
       </c>
       <c r="L261" s="11"/>
     </row>
-    <row r="262" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:12" ht="15.75">
       <c r="A262" s="3" t="s">
         <v>560</v>
       </c>
@@ -13051,7 +13049,7 @@
       </c>
       <c r="L262" s="11"/>
     </row>
-    <row r="263" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:12" ht="15.75">
       <c r="A263" s="3" t="s">
         <v>561</v>
       </c>
@@ -13079,7 +13077,7 @@
       </c>
       <c r="L263" s="11"/>
     </row>
-    <row r="264" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:12" ht="15.75">
       <c r="A264" s="3" t="s">
         <v>562</v>
       </c>
@@ -13107,7 +13105,7 @@
       </c>
       <c r="L264" s="11"/>
     </row>
-    <row r="265" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:12" ht="15.75">
       <c r="A265" s="3" t="s">
         <v>563</v>
       </c>
@@ -13135,7 +13133,7 @@
       </c>
       <c r="L265" s="11"/>
     </row>
-    <row r="266" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:12" ht="15.75">
       <c r="A266" s="3" t="s">
         <v>565</v>
       </c>
@@ -13163,7 +13161,7 @@
       </c>
       <c r="L266" s="11"/>
     </row>
-    <row r="267" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:12" ht="15.75">
       <c r="A267" s="3" t="s">
         <v>566</v>
       </c>
@@ -13191,7 +13189,7 @@
       </c>
       <c r="L267" s="11"/>
     </row>
-    <row r="268" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:12" ht="15.75">
       <c r="A268" s="3" t="s">
         <v>567</v>
       </c>
@@ -13219,7 +13217,7 @@
       </c>
       <c r="L268" s="11"/>
     </row>
-    <row r="269" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:12" ht="15.75">
       <c r="A269" s="3" t="s">
         <v>568</v>
       </c>
@@ -13247,7 +13245,7 @@
       </c>
       <c r="L269" s="11"/>
     </row>
-    <row r="270" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:12" ht="15.75">
       <c r="A270" s="3" t="s">
         <v>573</v>
       </c>
@@ -13275,7 +13273,7 @@
       </c>
       <c r="L270" s="11"/>
     </row>
-    <row r="271" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:12" ht="15.75">
       <c r="A271" s="3" t="s">
         <v>574</v>
       </c>
@@ -13303,7 +13301,7 @@
       </c>
       <c r="L271" s="11"/>
     </row>
-    <row r="272" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:12" ht="15.75">
       <c r="A272" s="3" t="s">
         <v>575</v>
       </c>
@@ -13331,7 +13329,7 @@
       </c>
       <c r="L272" s="11"/>
     </row>
-    <row r="273" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:12" ht="15.75">
       <c r="A273" s="3" t="s">
         <v>576</v>
       </c>
@@ -13359,7 +13357,7 @@
       </c>
       <c r="L273" s="11"/>
     </row>
-    <row r="274" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:12" ht="15.75">
       <c r="A274" s="3" t="s">
         <v>578</v>
       </c>
@@ -13387,7 +13385,7 @@
       </c>
       <c r="L274" s="11"/>
     </row>
-    <row r="275" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:12" ht="15.75">
       <c r="A275" s="3" t="s">
         <v>581</v>
       </c>
@@ -13415,7 +13413,7 @@
       </c>
       <c r="L275" s="11"/>
     </row>
-    <row r="276" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:12" ht="15.75">
       <c r="A276" s="3" t="s">
         <v>584</v>
       </c>
@@ -13443,7 +13441,7 @@
       </c>
       <c r="L276" s="11"/>
     </row>
-    <row r="277" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:12" ht="15.75">
       <c r="A277" s="3" t="s">
         <v>585</v>
       </c>
@@ -13471,7 +13469,7 @@
       </c>
       <c r="L277" s="11"/>
     </row>
-    <row r="278" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:12" ht="15.75">
       <c r="A278" s="3" t="s">
         <v>588</v>
       </c>
@@ -13499,7 +13497,7 @@
       </c>
       <c r="L278" s="11"/>
     </row>
-    <row r="279" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:12" ht="15.75">
       <c r="A279" s="3" t="s">
         <v>596</v>
       </c>
@@ -13527,7 +13525,7 @@
       </c>
       <c r="L279" s="11"/>
     </row>
-    <row r="280" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:12" ht="15.75">
       <c r="A280" s="3" t="s">
         <v>597</v>
       </c>
@@ -13555,7 +13553,7 @@
       </c>
       <c r="L280" s="11"/>
     </row>
-    <row r="281" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:12" ht="15.75">
       <c r="A281" s="3" t="s">
         <v>598</v>
       </c>
@@ -13583,7 +13581,7 @@
       </c>
       <c r="L281" s="11"/>
     </row>
-    <row r="282" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:12" ht="15.75">
       <c r="A282" s="3" t="s">
         <v>599</v>
       </c>
@@ -13611,7 +13609,7 @@
       </c>
       <c r="L282" s="11"/>
     </row>
-    <row r="283" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:12" ht="15.75">
       <c r="A283" s="3" t="s">
         <v>595</v>
       </c>
@@ -13639,7 +13637,7 @@
       </c>
       <c r="L283" s="11"/>
     </row>
-    <row r="284" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:12" ht="15.75">
       <c r="A284" s="3" t="s">
         <v>600</v>
       </c>
@@ -13667,7 +13665,7 @@
       </c>
       <c r="L284" s="11"/>
     </row>
-    <row r="285" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:12" ht="15.75">
       <c r="A285" s="3" t="s">
         <v>601</v>
       </c>
@@ -13695,7 +13693,7 @@
       </c>
       <c r="L285" s="11"/>
     </row>
-    <row r="286" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:12" ht="15.75">
       <c r="A286" s="3" t="s">
         <v>602</v>
       </c>
@@ -13723,7 +13721,7 @@
       </c>
       <c r="L286" s="11"/>
     </row>
-    <row r="287" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:12" ht="15.75">
       <c r="A287" s="3" t="s">
         <v>603</v>
       </c>
@@ -13751,7 +13749,7 @@
       </c>
       <c r="L287" s="11"/>
     </row>
-    <row r="288" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:12" ht="15.75">
       <c r="A288" s="3" t="s">
         <v>621</v>
       </c>
@@ -13779,7 +13777,7 @@
       </c>
       <c r="L288" s="11"/>
     </row>
-    <row r="289" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:12" ht="15.75">
       <c r="A289" s="3" t="s">
         <v>623</v>
       </c>
@@ -13807,7 +13805,7 @@
       </c>
       <c r="L289" s="11"/>
     </row>
-    <row r="290" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:12" ht="15.75">
       <c r="A290" s="3" t="s">
         <v>626</v>
       </c>
@@ -13835,7 +13833,7 @@
       </c>
       <c r="L290" s="11"/>
     </row>
-    <row r="291" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:12" ht="15.75">
       <c r="A291" s="3" t="s">
         <v>629</v>
       </c>
@@ -13863,7 +13861,7 @@
       </c>
       <c r="L291" s="11"/>
     </row>
-    <row r="292" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:12" ht="15.75">
       <c r="A292" s="3" t="s">
         <v>631</v>
       </c>
@@ -13891,7 +13889,7 @@
       </c>
       <c r="L292" s="11"/>
     </row>
-    <row r="293" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:12" ht="15.75">
       <c r="A293" s="3" t="s">
         <v>632</v>
       </c>
@@ -13919,7 +13917,7 @@
       </c>
       <c r="L293" s="11"/>
     </row>
-    <row r="294" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:12" ht="15.75">
       <c r="A294" s="3" t="s">
         <v>633</v>
       </c>
@@ -13947,7 +13945,7 @@
       </c>
       <c r="L294" s="11"/>
     </row>
-    <row r="295" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:12" ht="15.75">
       <c r="A295" s="3" t="s">
         <v>634</v>
       </c>
@@ -13975,7 +13973,7 @@
       </c>
       <c r="L295" s="11"/>
     </row>
-    <row r="296" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:12" ht="15.75">
       <c r="A296" s="3" t="s">
         <v>635</v>
       </c>
@@ -14003,7 +14001,7 @@
       </c>
       <c r="L296" s="11"/>
     </row>
-    <row r="297" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:12" ht="15.75">
       <c r="A297" s="3" t="s">
         <v>639</v>
       </c>
@@ -14031,7 +14029,7 @@
       </c>
       <c r="L297" s="11"/>
     </row>
-    <row r="298" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:12" ht="15.75">
       <c r="A298" s="3" t="s">
         <v>641</v>
       </c>
@@ -14059,7 +14057,7 @@
       </c>
       <c r="L298" s="11"/>
     </row>
-    <row r="299" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:12" ht="15.75">
       <c r="A299" s="3" t="s">
         <v>643</v>
       </c>
@@ -14087,7 +14085,7 @@
       </c>
       <c r="L299" s="11"/>
     </row>
-    <row r="300" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:12" ht="15.75">
       <c r="A300" s="3" t="s">
         <v>645</v>
       </c>
@@ -14115,7 +14113,7 @@
       </c>
       <c r="L300" s="11"/>
     </row>
-    <row r="301" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:12" ht="15.75">
       <c r="A301" s="3" t="s">
         <v>647</v>
       </c>
@@ -14143,7 +14141,7 @@
       </c>
       <c r="L301" s="11"/>
     </row>
-    <row r="302" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:12" ht="15.75">
       <c r="A302" s="3" t="s">
         <v>650</v>
       </c>
@@ -14171,7 +14169,7 @@
       </c>
       <c r="L302" s="11"/>
     </row>
-    <row r="303" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:12" ht="15.75">
       <c r="A303" s="3" t="s">
         <v>652</v>
       </c>
@@ -14199,7 +14197,7 @@
       </c>
       <c r="L303" s="11"/>
     </row>
-    <row r="304" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:12" ht="15.75">
       <c r="A304" s="3" t="s">
         <v>653</v>
       </c>
@@ -14227,7 +14225,7 @@
       </c>
       <c r="L304" s="11"/>
     </row>
-    <row r="305" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:12" ht="15.75">
       <c r="A305" s="3" t="s">
         <v>656</v>
       </c>
@@ -14255,7 +14253,7 @@
       </c>
       <c r="L305" s="11"/>
     </row>
-    <row r="306" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:12" ht="15.75">
       <c r="A306" s="3" t="s">
         <v>659</v>
       </c>
@@ -14283,7 +14281,7 @@
       </c>
       <c r="L306" s="11"/>
     </row>
-    <row r="307" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:12" ht="15.75">
       <c r="A307" s="3" t="s">
         <v>660</v>
       </c>
@@ -14311,7 +14309,7 @@
       </c>
       <c r="L307" s="11"/>
     </row>
-    <row r="308" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:12" ht="15.75">
       <c r="A308" s="3" t="s">
         <v>665</v>
       </c>
@@ -14339,7 +14337,7 @@
       </c>
       <c r="L308" s="11"/>
     </row>
-    <row r="309" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:12" ht="15.75">
       <c r="A309" s="3" t="s">
         <v>668</v>
       </c>
@@ -14367,7 +14365,7 @@
       </c>
       <c r="L309" s="11"/>
     </row>
-    <row r="310" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:12" ht="15.75">
       <c r="A310" s="3" t="s">
         <v>671</v>
       </c>
@@ -14395,7 +14393,7 @@
       </c>
       <c r="L310" s="11"/>
     </row>
-    <row r="311" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:12" ht="15.75">
       <c r="A311" s="3" t="s">
         <v>674</v>
       </c>
@@ -14423,7 +14421,7 @@
       </c>
       <c r="L311" s="11"/>
     </row>
-    <row r="312" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:12" ht="15.75">
       <c r="A312" s="3" t="s">
         <v>676</v>
       </c>
@@ -14451,7 +14449,7 @@
       </c>
       <c r="L312" s="11"/>
     </row>
-    <row r="313" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:12" ht="15.75">
       <c r="A313" s="3" t="s">
         <v>678</v>
       </c>
@@ -14479,7 +14477,7 @@
       </c>
       <c r="L313" s="11"/>
     </row>
-    <row r="314" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:12" ht="15.75">
       <c r="A314" s="3" t="s">
         <v>680</v>
       </c>
@@ -14507,7 +14505,7 @@
       </c>
       <c r="L314" s="11"/>
     </row>
-    <row r="315" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:12" ht="15.75">
       <c r="A315" s="3" t="s">
         <v>683</v>
       </c>
@@ -14535,7 +14533,7 @@
       </c>
       <c r="L315" s="11"/>
     </row>
-    <row r="316" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:12" ht="15.75">
       <c r="A316" s="3" t="s">
         <v>685</v>
       </c>
@@ -14563,7 +14561,7 @@
       </c>
       <c r="L316" s="11"/>
     </row>
-    <row r="317" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:12" ht="15.75">
       <c r="A317" s="3" t="s">
         <v>687</v>
       </c>
@@ -14591,7 +14589,7 @@
       </c>
       <c r="L317" s="11"/>
     </row>
-    <row r="318" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:12" ht="15.75">
       <c r="A318" s="3" t="s">
         <v>688</v>
       </c>
@@ -14619,7 +14617,7 @@
       </c>
       <c r="L318" s="11"/>
     </row>
-    <row r="319" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:12" ht="15.75">
       <c r="A319" s="3" t="s">
         <v>689</v>
       </c>
@@ -14647,7 +14645,7 @@
       </c>
       <c r="L319" s="11"/>
     </row>
-    <row r="320" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:12" ht="15.75">
       <c r="A320" s="3" t="s">
         <v>690</v>
       </c>
@@ -14675,7 +14673,7 @@
       </c>
       <c r="L320" s="11"/>
     </row>
-    <row r="321" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:12" ht="15.75">
       <c r="A321" s="3" t="s">
         <v>694</v>
       </c>
@@ -14703,7 +14701,7 @@
       </c>
       <c r="L321" s="11"/>
     </row>
-    <row r="322" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:12" ht="15.75">
       <c r="A322" s="3" t="s">
         <v>695</v>
       </c>
@@ -14731,7 +14729,7 @@
       </c>
       <c r="L322" s="11"/>
     </row>
-    <row r="323" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:12" ht="15.75">
       <c r="A323" s="3" t="s">
         <v>696</v>
       </c>
@@ -14759,7 +14757,7 @@
       </c>
       <c r="L323" s="11"/>
     </row>
-    <row r="324" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:12" ht="15.75">
       <c r="A324" s="3" t="s">
         <v>700</v>
       </c>
@@ -14787,7 +14785,7 @@
       </c>
       <c r="L324" s="11"/>
     </row>
-    <row r="325" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:12" ht="15.75">
       <c r="A325" s="3" t="s">
         <v>702</v>
       </c>
@@ -14815,7 +14813,7 @@
       </c>
       <c r="L325" s="11"/>
     </row>
-    <row r="326" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:12" ht="15.75">
       <c r="A326" s="3" t="s">
         <v>704</v>
       </c>
@@ -14843,7 +14841,7 @@
       </c>
       <c r="L326" s="11"/>
     </row>
-    <row r="327" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:12" ht="15.75">
       <c r="A327" s="3" t="s">
         <v>705</v>
       </c>
@@ -14871,7 +14869,7 @@
       </c>
       <c r="L327" s="11"/>
     </row>
-    <row r="328" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:12" ht="15.75">
       <c r="A328" s="3" t="s">
         <v>706</v>
       </c>
@@ -14899,7 +14897,7 @@
       </c>
       <c r="L328" s="11"/>
     </row>
-    <row r="329" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:12" ht="15.75">
       <c r="A329" s="3" t="s">
         <v>710</v>
       </c>
@@ -14927,7 +14925,7 @@
       </c>
       <c r="L329" s="11"/>
     </row>
-    <row r="330" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:12" ht="15.75">
       <c r="A330" s="3" t="s">
         <v>711</v>
       </c>
@@ -14955,7 +14953,7 @@
       </c>
       <c r="L330" s="11"/>
     </row>
-    <row r="331" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:12" ht="15.75">
       <c r="A331" s="3" t="s">
         <v>712</v>
       </c>
@@ -14983,7 +14981,7 @@
       </c>
       <c r="L331" s="11"/>
     </row>
-    <row r="332" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:12" ht="15.75">
       <c r="A332" s="3" t="s">
         <v>713</v>
       </c>
@@ -15011,7 +15009,7 @@
       </c>
       <c r="L332" s="11"/>
     </row>
-    <row r="333" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:12" ht="15.75">
       <c r="A333" s="3" t="s">
         <v>714</v>
       </c>
@@ -15039,7 +15037,7 @@
       </c>
       <c r="L333" s="11"/>
     </row>
-    <row r="334" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:12" ht="15.75">
       <c r="A334" s="3" t="s">
         <v>720</v>
       </c>
@@ -15067,7 +15065,7 @@
       </c>
       <c r="L334" s="11"/>
     </row>
-    <row r="335" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:12" ht="15.75">
       <c r="A335" s="3" t="s">
         <v>721</v>
       </c>
@@ -15095,7 +15093,7 @@
       </c>
       <c r="L335" s="11"/>
     </row>
-    <row r="336" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:12" ht="15.75">
       <c r="A336" s="3" t="s">
         <v>722</v>
       </c>
@@ -15123,7 +15121,7 @@
       </c>
       <c r="L336" s="11"/>
     </row>
-    <row r="337" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:12" ht="15.75">
       <c r="A337" s="3" t="s">
         <v>723</v>
       </c>
@@ -15151,7 +15149,7 @@
       </c>
       <c r="L337" s="11"/>
     </row>
-    <row r="338" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:12" ht="15.75">
       <c r="A338" s="3" t="s">
         <v>724</v>
       </c>
@@ -15179,7 +15177,7 @@
       </c>
       <c r="L338" s="11"/>
     </row>
-    <row r="339" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:12" ht="15.75">
       <c r="A339" s="3" t="s">
         <v>730</v>
       </c>
@@ -15207,7 +15205,7 @@
       </c>
       <c r="L339" s="11"/>
     </row>
-    <row r="340" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:12" ht="15.75">
       <c r="A340" s="3" t="s">
         <v>731</v>
       </c>
@@ -15235,7 +15233,7 @@
       </c>
       <c r="L340" s="11"/>
     </row>
-    <row r="341" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:12" ht="15.75">
       <c r="A341" s="3" t="s">
         <v>732</v>
       </c>
@@ -15263,7 +15261,7 @@
       </c>
       <c r="L341" s="11"/>
     </row>
-    <row r="342" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:12" ht="15.75">
       <c r="A342" s="3" t="s">
         <v>733</v>
       </c>
@@ -15291,7 +15289,7 @@
       </c>
       <c r="L342" s="11"/>
     </row>
-    <row r="343" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:12" ht="15.75">
       <c r="A343" s="3" t="s">
         <v>734</v>
       </c>
@@ -15319,7 +15317,7 @@
       </c>
       <c r="L343" s="11"/>
     </row>
-    <row r="344" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:12" ht="15.75">
       <c r="A344" s="3" t="s">
         <v>740</v>
       </c>
@@ -15347,7 +15345,7 @@
       </c>
       <c r="L344" s="11"/>
     </row>
-    <row r="345" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:12" ht="15.75">
       <c r="A345" s="3" t="s">
         <v>741</v>
       </c>
@@ -15375,7 +15373,7 @@
       </c>
       <c r="L345" s="11"/>
     </row>
-    <row r="346" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:12" ht="15.75">
       <c r="A346" s="3" t="s">
         <v>742</v>
       </c>
@@ -15403,7 +15401,7 @@
       </c>
       <c r="L346" s="11"/>
     </row>
-    <row r="347" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:12" ht="15.75">
       <c r="A347" s="3" t="s">
         <v>743</v>
       </c>
@@ -15431,7 +15429,7 @@
       </c>
       <c r="L347" s="11"/>
     </row>
-    <row r="348" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:12" ht="15.75">
       <c r="A348" s="3" t="s">
         <v>744</v>
       </c>
@@ -15459,7 +15457,7 @@
       </c>
       <c r="L348" s="11"/>
     </row>
-    <row r="349" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:12" ht="15.75">
       <c r="A349" s="3" t="s">
         <v>197</v>
       </c>
@@ -15487,7 +15485,7 @@
       </c>
       <c r="L349" s="11"/>
     </row>
-    <row r="350" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:12" ht="15.75">
       <c r="A350" s="3" t="s">
         <v>751</v>
       </c>
@@ -15515,7 +15513,7 @@
       </c>
       <c r="L350" s="11"/>
     </row>
-    <row r="351" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:12" ht="15.75">
       <c r="A351" s="3" t="s">
         <v>753</v>
       </c>
@@ -15543,7 +15541,7 @@
       </c>
       <c r="L351" s="11"/>
     </row>
-    <row r="352" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:12" ht="15.75">
       <c r="A352" s="3" t="s">
         <v>755</v>
       </c>
@@ -15571,7 +15569,7 @@
       </c>
       <c r="L352" s="11"/>
     </row>
-    <row r="353" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:12" ht="15.75">
       <c r="A353" s="3" t="s">
         <v>756</v>
       </c>
@@ -15599,7 +15597,7 @@
       </c>
       <c r="L353" s="11"/>
     </row>
-    <row r="354" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:12" ht="15.75">
       <c r="A354" s="3" t="s">
         <v>759</v>
       </c>
@@ -15627,7 +15625,7 @@
       </c>
       <c r="L354" s="11"/>
     </row>
-    <row r="355" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:12" ht="15.75">
       <c r="A355" s="3" t="s">
         <v>760</v>
       </c>
@@ -15655,7 +15653,7 @@
       </c>
       <c r="L355" s="11"/>
     </row>
-    <row r="356" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:12" ht="15.75">
       <c r="A356" s="3" t="s">
         <v>763</v>
       </c>
@@ -15683,7 +15681,7 @@
       </c>
       <c r="L356" s="11"/>
     </row>
-    <row r="357" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:12" ht="15.75">
       <c r="A357" s="3" t="s">
         <v>764</v>
       </c>
@@ -15711,7 +15709,7 @@
       </c>
       <c r="L357" s="11"/>
     </row>
-    <row r="358" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:12" ht="15.75">
       <c r="A358" s="3" t="s">
         <v>769</v>
       </c>
@@ -15736,7 +15734,7 @@
       </c>
       <c r="L358" s="11"/>
     </row>
-    <row r="359" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:12" ht="15.75">
       <c r="A359" s="3" t="s">
         <v>771</v>
       </c>
@@ -15764,7 +15762,7 @@
       </c>
       <c r="L359" s="11"/>
     </row>
-    <row r="360" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:12" ht="15.75">
       <c r="A360" s="3" t="s">
         <v>774</v>
       </c>
@@ -15792,7 +15790,7 @@
       </c>
       <c r="L360" s="11"/>
     </row>
-    <row r="361" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:12" ht="15.75">
       <c r="A361" s="3" t="s">
         <v>778</v>
       </c>
@@ -15820,7 +15818,7 @@
       </c>
       <c r="L361" s="11"/>
     </row>
-    <row r="362" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:12" ht="15.75">
       <c r="A362" s="3" t="s">
         <v>781</v>
       </c>
@@ -15848,7 +15846,7 @@
       </c>
       <c r="L362" s="11"/>
     </row>
-    <row r="363" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:12" ht="15.75">
       <c r="A363" s="3" t="s">
         <v>784</v>
       </c>
@@ -15876,7 +15874,7 @@
       </c>
       <c r="L363" s="11"/>
     </row>
-    <row r="364" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:12" ht="15.75">
       <c r="A364" s="3" t="s">
         <v>787</v>
       </c>
@@ -15904,7 +15902,7 @@
       </c>
       <c r="L364" s="11"/>
     </row>
-    <row r="365" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:12" ht="15.75">
       <c r="A365" s="3" t="s">
         <v>789</v>
       </c>
@@ -15932,7 +15930,7 @@
       </c>
       <c r="L365" s="11"/>
     </row>
-    <row r="366" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:12" ht="15.75">
       <c r="A366" s="3" t="s">
         <v>792</v>
       </c>
@@ -15960,7 +15958,7 @@
       </c>
       <c r="L366" s="11"/>
     </row>
-    <row r="367" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:12" ht="15.75">
       <c r="A367" s="3" t="s">
         <v>795</v>
       </c>
@@ -15988,7 +15986,7 @@
       </c>
       <c r="L367" s="11"/>
     </row>
-    <row r="368" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:12" ht="15.75">
       <c r="A368" s="3" t="s">
         <v>798</v>
       </c>
@@ -16016,7 +16014,7 @@
       </c>
       <c r="L368" s="11"/>
     </row>
-    <row r="369" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:12" ht="15.75">
       <c r="A369" s="3" t="s">
         <v>802</v>
       </c>
@@ -16047,7 +16045,7 @@
       </c>
       <c r="L369" s="11"/>
     </row>
-    <row r="370" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:12" ht="15.75">
       <c r="A370" s="3" t="s">
         <v>803</v>
       </c>
@@ -16075,7 +16073,7 @@
       </c>
       <c r="L370" s="11"/>
     </row>
-    <row r="371" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:12" ht="15.75">
       <c r="A371" s="3" t="s">
         <v>806</v>
       </c>
@@ -16103,7 +16101,7 @@
       </c>
       <c r="L371" s="11"/>
     </row>
-    <row r="372" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:12" ht="15.75">
       <c r="A372" s="3" t="s">
         <v>809</v>
       </c>
@@ -16131,7 +16129,7 @@
       </c>
       <c r="L372" s="11"/>
     </row>
-    <row r="373" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:12" ht="15.75">
       <c r="A373" s="3" t="s">
         <v>812</v>
       </c>
@@ -16159,7 +16157,7 @@
       </c>
       <c r="L373" s="11"/>
     </row>
-    <row r="374" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:12" ht="15.75">
       <c r="A374" s="3" t="s">
         <v>816</v>
       </c>
@@ -16187,7 +16185,7 @@
       </c>
       <c r="L374" s="11"/>
     </row>
-    <row r="375" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:12" ht="15.75">
       <c r="A375" s="3" t="s">
         <v>817</v>
       </c>
@@ -16215,7 +16213,7 @@
       </c>
       <c r="L375" s="11"/>
     </row>
-    <row r="376" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:12" ht="15.75">
       <c r="A376" s="3" t="s">
         <v>818</v>
       </c>
@@ -16246,7 +16244,7 @@
       </c>
       <c r="L376" s="11"/>
     </row>
-    <row r="377" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:12" ht="15.75">
       <c r="A377" s="3" t="s">
         <v>819</v>
       </c>
@@ -16274,7 +16272,7 @@
       </c>
       <c r="L377" s="11"/>
     </row>
-    <row r="378" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:12" ht="15.75">
       <c r="A378" s="3" t="s">
         <v>820</v>
       </c>
@@ -16302,7 +16300,7 @@
       </c>
       <c r="L378" s="11"/>
     </row>
-    <row r="379" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:12" ht="15.75">
       <c r="A379" s="3" t="s">
         <v>821</v>
       </c>
@@ -16330,7 +16328,7 @@
       </c>
       <c r="L379" s="11"/>
     </row>
-    <row r="380" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:12" ht="15.75">
       <c r="A380" s="3" t="s">
         <v>822</v>
       </c>
@@ -16358,7 +16356,7 @@
       </c>
       <c r="L380" s="11"/>
     </row>
-    <row r="381" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:12" ht="15.75">
       <c r="A381" s="3" t="s">
         <v>831</v>
       </c>
@@ -16386,7 +16384,7 @@
       </c>
       <c r="L381" s="11"/>
     </row>
-    <row r="382" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:12" ht="15.75">
       <c r="A382" s="3" t="s">
         <v>832</v>
       </c>
@@ -16414,7 +16412,7 @@
       </c>
       <c r="L382" s="11"/>
     </row>
-    <row r="383" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:12" ht="15.75">
       <c r="A383" s="3" t="s">
         <v>833</v>
       </c>
@@ -16442,7 +16440,7 @@
       </c>
       <c r="L383" s="11"/>
     </row>
-    <row r="384" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:12" ht="15.75">
       <c r="A384" s="3" t="s">
         <v>834</v>
       </c>
@@ -16470,7 +16468,7 @@
       </c>
       <c r="L384" s="11"/>
     </row>
-    <row r="385" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:12" ht="15.75">
       <c r="A385" s="3" t="s">
         <v>835</v>
       </c>
@@ -16498,7 +16496,7 @@
       </c>
       <c r="L385" s="11"/>
     </row>
-    <row r="386" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:12" ht="15.75">
       <c r="A386" s="3" t="s">
         <v>841</v>
       </c>
@@ -16526,7 +16524,7 @@
       </c>
       <c r="L386" s="11"/>
     </row>
-    <row r="387" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:12" ht="15.75">
       <c r="A387" s="3" t="s">
         <v>845</v>
       </c>
@@ -16554,7 +16552,7 @@
       </c>
       <c r="L387" s="11"/>
     </row>
-    <row r="388" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:12" ht="15.75">
       <c r="A388" s="3" t="s">
         <v>848</v>
       </c>
@@ -16582,7 +16580,7 @@
       </c>
       <c r="L388" s="11"/>
     </row>
-    <row r="389" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:12" ht="15.75">
       <c r="A389" s="3" t="s">
         <v>849</v>
       </c>
@@ -16610,7 +16608,7 @@
       </c>
       <c r="L389" s="11"/>
     </row>
-    <row r="390" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:12" ht="15.75">
       <c r="A390" s="3" t="s">
         <v>850</v>
       </c>
@@ -16638,7 +16636,7 @@
       </c>
       <c r="L390" s="11"/>
     </row>
-    <row r="391" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:12" ht="15.75">
       <c r="A391" s="3" t="s">
         <v>852</v>
       </c>
@@ -16666,7 +16664,7 @@
       </c>
       <c r="L391" s="11"/>
     </row>
-    <row r="392" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:12" ht="15.75">
       <c r="A392" s="3" t="s">
         <v>855</v>
       </c>
@@ -16694,7 +16692,7 @@
       </c>
       <c r="L392" s="11"/>
     </row>
-    <row r="393" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:12" ht="15.75">
       <c r="A393" s="3" t="s">
         <v>201</v>
       </c>
@@ -16722,7 +16720,7 @@
       </c>
       <c r="L393" s="11"/>
     </row>
-    <row r="394" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:12" ht="15.75">
       <c r="A394" s="3" t="s">
         <v>857</v>
       </c>
@@ -16750,7 +16748,7 @@
       </c>
       <c r="L394" s="11"/>
     </row>
-    <row r="395" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:12" ht="15.75">
       <c r="A395" s="3" t="s">
         <v>859</v>
       </c>
@@ -16778,7 +16776,7 @@
       </c>
       <c r="L395" s="11"/>
     </row>
-    <row r="396" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:12" ht="15.75">
       <c r="A396" s="3" t="s">
         <v>862</v>
       </c>
@@ -16806,7 +16804,7 @@
       </c>
       <c r="L396" s="11"/>
     </row>
-    <row r="397" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:12" ht="15.75">
       <c r="A397" s="3" t="s">
         <v>863</v>
       </c>
@@ -16834,7 +16832,7 @@
       </c>
       <c r="L397" s="11"/>
     </row>
-    <row r="398" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:12" ht="15.75">
       <c r="A398" s="3" t="s">
         <v>866</v>
       </c>
@@ -16862,7 +16860,7 @@
       </c>
       <c r="L398" s="11"/>
     </row>
-    <row r="399" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:12" ht="15.75">
       <c r="A399" s="3" t="s">
         <v>868</v>
       </c>
@@ -16890,7 +16888,7 @@
       </c>
       <c r="L399" s="11"/>
     </row>
-    <row r="400" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:12" ht="15.75">
       <c r="A400" s="3" t="s">
         <v>869</v>
       </c>
@@ -16918,7 +16916,7 @@
       </c>
       <c r="L400" s="11"/>
     </row>
-    <row r="401" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:12" ht="15.75">
       <c r="A401" s="3" t="s">
         <v>872</v>
       </c>
@@ -16946,7 +16944,7 @@
       </c>
       <c r="L401" s="11"/>
     </row>
-    <row r="402" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:12" ht="15.75">
       <c r="A402" s="3" t="s">
         <v>874</v>
       </c>
@@ -16977,7 +16975,7 @@
       </c>
       <c r="L402" s="11"/>
     </row>
-    <row r="403" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:12" ht="15.75">
       <c r="A403" s="3" t="s">
         <v>876</v>
       </c>
@@ -17005,7 +17003,7 @@
       </c>
       <c r="L403" s="11"/>
     </row>
-    <row r="404" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:12" ht="15.75">
       <c r="A404" s="3" t="s">
         <v>878</v>
       </c>
@@ -17036,7 +17034,7 @@
       </c>
       <c r="L404" s="11"/>
     </row>
-    <row r="405" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:12" ht="15.75">
       <c r="A405" s="3" t="s">
         <v>880</v>
       </c>
@@ -17064,7 +17062,7 @@
       </c>
       <c r="L405" s="11"/>
     </row>
-    <row r="406" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:12" ht="15.75">
       <c r="A406" s="3" t="s">
         <v>882</v>
       </c>
@@ -17095,7 +17093,7 @@
       </c>
       <c r="L406" s="11"/>
     </row>
-    <row r="407" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:12" ht="15.75">
       <c r="A407" s="3" t="s">
         <v>884</v>
       </c>
@@ -17123,7 +17121,7 @@
       </c>
       <c r="L407" s="11"/>
     </row>
-    <row r="408" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:12" ht="15.75">
       <c r="A408" s="3" t="s">
         <v>886</v>
       </c>
@@ -17151,7 +17149,7 @@
       </c>
       <c r="L408" s="11"/>
     </row>
-    <row r="409" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:12" ht="15.75">
       <c r="A409" s="3" t="s">
         <v>888</v>
       </c>
@@ -17179,7 +17177,7 @@
       </c>
       <c r="L409" s="11"/>
     </row>
-    <row r="410" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:12" ht="15.75">
       <c r="A410" s="3" t="s">
         <v>889</v>
       </c>
@@ -17207,7 +17205,7 @@
       </c>
       <c r="L410" s="11"/>
     </row>
-    <row r="411" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:12" ht="15.75">
       <c r="A411" s="3" t="s">
         <v>890</v>
       </c>
@@ -17235,7 +17233,7 @@
       </c>
       <c r="L411" s="11"/>
     </row>
-    <row r="412" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:12" ht="15.75">
       <c r="A412" s="3" t="s">
         <v>894</v>
       </c>
@@ -17263,7 +17261,7 @@
       </c>
       <c r="L412" s="11"/>
     </row>
-    <row r="413" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:12" ht="15.75">
       <c r="A413" s="3" t="s">
         <v>895</v>
       </c>
@@ -17291,7 +17289,7 @@
       </c>
       <c r="L413" s="11"/>
     </row>
-    <row r="414" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:12" ht="15.75">
       <c r="A414" s="3" t="s">
         <v>896</v>
       </c>
@@ -17319,7 +17317,7 @@
       </c>
       <c r="L414" s="11"/>
     </row>
-    <row r="415" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:12" ht="15.75">
       <c r="A415" s="3" t="s">
         <v>897</v>
       </c>
@@ -17347,7 +17345,7 @@
       </c>
       <c r="L415" s="11"/>
     </row>
-    <row r="416" spans="1:12" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:12" ht="15.75">
       <c r="A416" s="3" t="s">
         <v>902</v>
       </c>
@@ -17375,7 +17373,7 @@
       </c>
       <c r="L416" s="11"/>
     </row>
-    <row r="417" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:16" ht="15.75">
       <c r="A417" s="3" t="s">
         <v>903</v>
       </c>
@@ -17403,7 +17401,7 @@
       </c>
       <c r="L417" s="11"/>
     </row>
-    <row r="418" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:16" ht="15.75">
       <c r="A418" s="3" t="s">
         <v>904</v>
       </c>
@@ -17431,7 +17429,7 @@
       </c>
       <c r="L418" s="11"/>
     </row>
-    <row r="419" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:16" ht="15.75">
       <c r="A419" s="3" t="s">
         <v>905</v>
       </c>
@@ -17459,7 +17457,7 @@
       </c>
       <c r="L419" s="11"/>
     </row>
-    <row r="420" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:16" ht="15.75">
       <c r="A420" s="3" t="s">
         <v>910</v>
       </c>
@@ -17487,7 +17485,7 @@
       </c>
       <c r="L420" s="11"/>
     </row>
-    <row r="421" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:16" ht="15.75">
       <c r="A421" s="3" t="s">
         <v>911</v>
       </c>
@@ -17515,7 +17513,7 @@
       </c>
       <c r="L421" s="11"/>
     </row>
-    <row r="422" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:16" ht="15.75">
       <c r="A422" s="3" t="s">
         <v>912</v>
       </c>
@@ -17543,7 +17541,7 @@
       </c>
       <c r="L422" s="11"/>
     </row>
-    <row r="423" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:16" ht="15.75">
       <c r="A423" s="3" t="s">
         <v>913</v>
       </c>
@@ -17571,7 +17569,7 @@
       </c>
       <c r="L423" s="11"/>
     </row>
-    <row r="424" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:16" ht="15.75">
       <c r="A424" s="3" t="s">
         <v>967</v>
       </c>
@@ -17616,7 +17614,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="425" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:16" ht="15.75">
       <c r="A425" s="3" t="s">
         <v>922</v>
       </c>
@@ -17644,7 +17642,7 @@
       </c>
       <c r="L425" s="11"/>
     </row>
-    <row r="426" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:16" ht="15.75">
       <c r="A426" s="3" t="s">
         <v>924</v>
       </c>
@@ -17672,7 +17670,7 @@
       </c>
       <c r="L426" s="11"/>
     </row>
-    <row r="427" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:16" ht="15.75">
       <c r="A427" s="3" t="s">
         <v>926</v>
       </c>
@@ -17700,7 +17698,7 @@
       </c>
       <c r="L427" s="11"/>
     </row>
-    <row r="428" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:16" ht="15.75">
       <c r="A428" s="3" t="s">
         <v>929</v>
       </c>
@@ -17728,7 +17726,7 @@
       </c>
       <c r="L428" s="11"/>
     </row>
-    <row r="429" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:16" ht="15.75">
       <c r="A429" s="3" t="s">
         <v>932</v>
       </c>
@@ -17756,7 +17754,7 @@
       </c>
       <c r="L429" s="11"/>
     </row>
-    <row r="430" spans="1:16" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:16" ht="15.75">
       <c r="A430" s="3" t="s">
         <v>935</v>
       </c>
@@ -17791,24 +17789,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>